<commit_message>
añadiendo diagrama de gantt
</commit_message>
<xml_diff>
--- a/assets/Plan de trabajo.xlsx
+++ b/assets/Plan de trabajo.xlsx
@@ -1360,7 +1360,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="23">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
@@ -1392,8 +1392,8 @@
       <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="23">
-        <v>0.0</v>
+      <c r="D21" s="17">
+        <v>1.0</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
@@ -1409,7 +1409,7 @@
         <v>23</v>
       </c>
       <c r="D22" s="23">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
@@ -1427,7 +1427,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="23">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
@@ -1442,8 +1442,8 @@
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="23">
-        <v>0.0</v>
+      <c r="D24" s="17">
+        <v>1.0</v>
       </c>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
@@ -1458,8 +1458,8 @@
       <c r="C25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="23">
-        <v>0.0</v>
+      <c r="D25" s="17">
+        <v>1.0</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
@@ -1476,8 +1476,8 @@
       <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="23">
-        <v>0.0</v>
+      <c r="D26" s="17">
+        <v>1.0</v>
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
@@ -1492,8 +1492,8 @@
       <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="23">
-        <v>0.0</v>
+      <c r="D27" s="17">
+        <v>1.0</v>
       </c>
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
@@ -1508,8 +1508,8 @@
       <c r="C28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="23">
-        <v>0.0</v>
+      <c r="D28" s="17">
+        <v>1.0</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -1524,8 +1524,8 @@
       <c r="C29" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="23">
-        <v>0.0</v>
+      <c r="D29" s="17">
+        <v>1.0</v>
       </c>
       <c r="N29" s="26"/>
     </row>

</xml_diff>